<commit_message>
Added system architecture flow charts
</commit_message>
<xml_diff>
--- a/docs/Robot_BOM.xlsx
+++ b/docs/Robot_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan Heddle\OneDrive\Desktop\Ergos-Dynamic-Humanoid-Platform\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC17398-611D-4B36-81C8-E0BF1E97DA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CF7321-4CC5-4A11-9E0E-015C31A4BDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02CBD0F1-74CF-4889-91DA-ED3C1ACE063A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02CBD0F1-74CF-4889-91DA-ED3C1ACE063A}"/>
   </bookViews>
   <sheets>
     <sheet name="Robot_BOM" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Part</t>
   </si>
@@ -95,24 +95,12 @@
     <t>https://www.amazon.ca/uxcell-Bearings-8x12x3-5mm-Miniature-Precision/dp/B0CM6G9ZKZ/ref=sr_1_1_sspa?dib=eyJ2IjoiMSJ9.ONfxX4N7YaB0nVC5ooFVR9CCxoUVbn3Br9jtOb0-Fo-zE4gYb88mbb66dYdjR6gEh627goLwYuHMomYA8kvUzXY5DLMQVPKuphA9umCSnN3MVsYfZ0Slrq8DpGwK5CRvT642U1hslR5yB0lF6-7GzffSewLB3gidbmBOtkR1I4Ivj7Z_WzG7EQqdRQJ02oESFyH8raAOuMqorI80Kgayp6weuZ9eShOwDAKoS15ux2j5g-CLD59jPmMMhaawTZks89mpoJ57szjD-dOtKGzWbOD8rqQywYYn53n3Uu-fQ6M.9KLB09EZX1ib8fGp-LBSh-REjrEpmcf8nIA4aD85yos&amp;dib_tag=se&amp;keywords=MR128&amp;qid=1757789974&amp;sr=8-1-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;th=1</t>
   </si>
   <si>
-    <t>https://www.amazon.ca/Washer-Stainless-Steel-Thickness-Finish/dp/B07WZ5WQCG/ref=sr_1_10?crid=320K0U2K9QBJT&amp;dib=eyJ2IjoiMSJ9.bU4WlhE01AOwri_ZiS-jaT3dgrPXs_mB6DBURF6A_iXxHzcvqoDcLQi9Yo4pApIToxzPWJEICIk6kfGcPPw5o2ChnMWoIQ4tMY4ZjIKkt4Lmg-vSwSAAxdh5hPv71Pnt20osVIyV8ATOBfxV5-QbIqpO3LvGZZ5eg7c_Goz0zkv-BnaugJhgxOrfqDl9txpuqVW-MD6GOQsfIIX7DL6BYa9BPiH2iUuowKyYwXHyQwd_gRB2PAUffi27DmjUU1UIKkUuAs-D_9yoEWNk7gzVQB7HvEo4Wzn_NqQep9eqLAA.JMeExjSa2y9wntmVUC982gLpv5xwGaR47xbU7DAM7Lw&amp;dib_tag=se&amp;keywords=washer%2B5mm%2Bid&amp;qid=1757896497&amp;sprefix=washer%2B5mm%2Bid%2Caps%2C121&amp;sr=8-10&amp;th=1</t>
-  </si>
-  <si>
-    <t>5mm ID Washers</t>
-  </si>
-  <si>
     <t>ELECTRICAL</t>
   </si>
   <si>
     <t>SOFTWARE</t>
   </si>
   <si>
-    <t>KingSpec SSD 256GB</t>
-  </si>
-  <si>
-    <t>amazon.ca/KingSpec-256GB-NVMe-Gen3x4-2280/dp/B0D1R7HDJF/ref=sr_1_4_sspa?dib=eyJ2IjoiMSJ9.drCI5nIcaeNPjaX0FtDF8yDeVSCMk-LPA48gHaRXe-cwVGWjCxJL65svHmyg2GuNviJJjFMHFxqtPFsTPqbO8bDCQYAhLulUPzHajsa3qesuBG-68gf9MmxxEQI9xvIyFkV3aeJVHZMG5ffkCe9Tqw8MiElN7i4kqwH-8EZQrt2HO-BxyOtqeZatRlNgWBmbXY8k62EmUHwDqehHjMhGfUWCrvhPX4iFZzs07Gf1AJohVQDiR77IHLYDGFK7Irg7midqELnI0DR43ZaOOK73QskIxV0fFIiUJCUgiiwTcD0.XDUgV00pV5rFfMhkjRa5oZUwf0awBMF0YZ8svnmxo-8&amp;dib_tag=se&amp;keywords=nvme+m4+128gb&amp;qid=1757962271&amp;sr=8-4-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;psc=1</t>
-  </si>
-  <si>
     <t>Loctite 638</t>
   </si>
   <si>
@@ -146,15 +134,9 @@
     <t>Used to reduce axial friction and prevent rubbing between rotating parts and stationary brackets.</t>
   </si>
   <si>
-    <t>Precision bearings supporting rotating shafts at each joint to minimize friction and improve motion stability.</t>
-  </si>
-  <si>
     <t>Smaller bearings used in compact joint housings where load and speed requirements are moderate.</t>
   </si>
   <si>
-    <t>Provide spacing and distribute load in smaller shaft assemblies, preventing wear on rotating components.</t>
-  </si>
-  <si>
     <t>High-strength retaining compound for securing shafts, pulleys, and bearings, preventing slippage under dynamic loads.</t>
   </si>
   <si>
@@ -209,16 +191,16 @@
     <t>https://www.aliexpress.com/item/1005009686443539.html?spm=a2g0o.order_list.order_list_main.5.1bdb1802M7naAb</t>
   </si>
   <si>
-    <t>MR148 Bearings</t>
-  </si>
-  <si>
-    <t>https://www.amazon.ca/uxcell-Shielded-Bearings-Electric-Skateboards/dp/B0F4XQMKXS/ref=sr_1_1_sspa?dib=eyJ2IjoiMSJ9.Ka430sxQAP04OoBK47h1qKXm3S2enh3rolkJHXz1D3zydpC8S0LXio9RFsMlwfRKQjU7mNFfzdzJ9uyESOFIz_8CuTr-PB7EgF0Kn2RnIizELQTFnxx_dkN8ryx4gxgBSzyyZzOU6qKEAfu3LLHya2Vs0HoFxbMBoA9wryOU0oVG5YL-keJnCd_D6FYYFZy1Xat7auU4XKdTJJtnUCTj_ID38tkZr1wIKQ2llHJTx7YshIiA6dGD3eP0ys2AQmA_9M0cCjFr5wDeJ2bJKckJWv-ooM8LhTDVAocMyR0ulgk.IeznUwyVaf1LQ8avqikrcNcATYaXNyILqJUt5nNtcwA&amp;dib_tag=se&amp;keywords=bearing%2BID%2B8mm%2B14mm%2BOD&amp;qid=1765240309&amp;sr=8-1-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;th=1</t>
-  </si>
-  <si>
     <t>8mm ID 11 mm OD Washers</t>
   </si>
   <si>
     <t>https://www.gobilda.com/2807-series-stainless-steel-shim-8mm-id-x-11mm-od-0-25mm-thickness-12-pack/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/dp/B0D4RD18YV?ref=ppx_yo2ov_dt_b_fed_asin_title&amp;th=1</t>
+  </si>
+  <si>
+    <t>Patriot P320 128GB SSD</t>
   </si>
 </sst>
 </file>
@@ -349,99 +331,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>22887</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>325335</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>45576</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>226440</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6FF1952-ABB6-BC18-7D1A-48DB9DE8B662}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14922708" y="4434692"/>
-          <a:ext cx="6758225" cy="3751927"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>100487</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>247475</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>345513</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>256381</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2052A685-CEED-FE37-4C12-24046AB0CB5E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15004311" y="718122"/>
-          <a:ext cx="5691084" cy="3639612"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -764,7 +653,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -812,8 +701,8 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="8">
-        <f>SUM(F3:F38)</f>
-        <v>2784.1956999999998</v>
+        <f>SUM(F3:F36)</f>
+        <v>2960.0236999999997</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -824,7 +713,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>14</v>
@@ -833,7 +722,7 @@
         <v>65.81</v>
       </c>
       <c r="F3" s="4">
-        <f t="shared" ref="F3:F10" si="0">(D3*E3)*1.13</f>
+        <f t="shared" ref="F3:F9" si="0">(D3*E3)*1.13</f>
         <v>1041.1142</v>
       </c>
     </row>
@@ -845,7 +734,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -866,7 +755,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -881,13 +770,13 @@
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -902,13 +791,13 @@
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -923,13 +812,13 @@
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -944,266 +833,230 @@
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" s="4">
-        <v>16.489999999999998</v>
+        <v>16.29</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="0"/>
-        <v>18.633699999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>18.407699999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="4">
-        <v>16.29</v>
+        <v>44.99</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="0"/>
-        <v>18.407699999999998</v>
+        <f>(D10*E10)*1.13</f>
+        <v>101.67739999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>24</v>
+      </c>
+      <c r="F11" s="4">
+        <f>(D11*E11)*1.13</f>
+        <v>27.119999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <f t="shared" ref="F14:F18" si="1">(D14*E14)*1.13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>99.99</v>
+      </c>
+      <c r="F15" s="4">
+        <f>(D15*E15)*1.13</f>
+        <v>112.98869999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>284</v>
+      </c>
+      <c r="F16" s="4">
+        <f>(D16*E16)*1.13</f>
+        <v>320.91999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>38</v>
       </c>
-      <c r="F11">
-        <f t="shared" ref="F11:F20" si="1">(D11*E11)*1.13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4">
-        <v>44.99</v>
-      </c>
-      <c r="F12" s="4">
-        <f>(D12*E12)*1.13</f>
-        <v>101.67739999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D13">
+      <c r="D17">
         <v>1</v>
       </c>
-      <c r="E13" s="5">
-        <v>24</v>
-      </c>
-      <c r="F13" s="4">
-        <f>(D13*E13)*1.13</f>
-        <v>27.119999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2">
+      <c r="E17" s="5">
+        <v>183</v>
+      </c>
+      <c r="F17" s="4">
+        <f>(D17*E17)*1.13</f>
+        <v>206.79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="6"/>
+      <c r="F18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21">
         <v>1</v>
       </c>
-      <c r="E17" s="4">
-        <v>99.99</v>
-      </c>
-      <c r="F17" s="4">
-        <f>(D17*E17)*1.13</f>
-        <v>112.98869999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18">
+      <c r="E21" s="4">
+        <v>344.95</v>
+      </c>
+      <c r="F21" s="4">
+        <f>(D21*E21)*1.13</f>
+        <v>389.79349999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22">
         <v>1</v>
       </c>
-      <c r="E18" s="4">
-        <v>126.91</v>
-      </c>
-      <c r="F18" s="4">
-        <f>(D18*E18)*1.13</f>
-        <v>143.40829999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5">
-        <v>183</v>
-      </c>
-      <c r="F19" s="4">
-        <f>(D19*E19)*1.13</f>
-        <v>206.79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="6"/>
-      <c r="F20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="5">
+        <v>146.84</v>
+      </c>
+      <c r="F22" s="4">
+        <f>(D22*E22)*1.13</f>
+        <v>165.92919999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" s="4">
-        <v>344.95</v>
+        <v>47.99</v>
       </c>
       <c r="F23" s="4">
         <f>(D23*E23)*1.13</f>
-        <v>389.79349999999994</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="5">
-        <v>146.84</v>
-      </c>
-      <c r="F24" s="4">
-        <f>(D24*E24)*1.13</f>
-        <v>165.92919999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" s="4">
-        <v>32.99</v>
-      </c>
-      <c r="F25" s="4">
-        <f>(D25*E25)*1.13</f>
-        <v>37.278700000000001</v>
+        <v>54.228699999999996</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1213,19 +1066,18 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{ABAF853C-7614-4C43-8D02-3509970FF289}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{81C68F65-402F-485A-8246-28C1ED3C194F}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{568D074D-A623-41D8-A536-15D5A113AF52}"/>
-    <hyperlink ref="B23" r:id="rId4" display="https://www.amazon.ca/NVIDIA-Jetson-Orin-Nano-Developer/dp/B0BZJTQ5YP/ref=sr_1_5?dib=eyJ2IjoiMSJ9.oBPmo8N1125w9UZ8-xtxgBB0vzdg_OFiDKOJUmUak3KsGol2xTi80fCYUWqHlOGe2kAe8ESSo6BWqINztXDYxQeYiaTolbh4JB0c7Y3jwzqBn2JFR0HiK1FyJ5kyFpPhXSp1aJv5xMC--j8b-fNhdLSSJwvjbd0XY8EXhorkOxJFMnOfcD0O0oLoypf_Fx_o_Mmr-y09hK1oqRhDgOKDMI8MH5wdi7HBtWLImeM1blm4-70toRIjqXFsuk1DjbODSwJutIPBQJ3qrJjQuqE5pt5imxUwUY1I2YieMJwjEhU.iMrYs9zK_mCJTvqh5PRE7PjCeBtP2gORpf3H3tjRj9Q&amp;dib_tag=se&amp;keywords=jetson+orin+nano+dev+kit&amp;qid=1759703130&amp;sr=8-5" xr:uid="{1292E30F-6024-4A1A-B37C-1DA10F1BD571}"/>
-    <hyperlink ref="B24" r:id="rId5" xr:uid="{570B946F-A3F9-46CD-89E7-C74FEE892AE5}"/>
-    <hyperlink ref="B12" r:id="rId6" display="Amazon" xr:uid="{41208C38-E731-44F2-BEE2-61FCB8EB62DA}"/>
-    <hyperlink ref="B17" r:id="rId7" display="https://www.amazon.ca/DXF-Battery-Hardcase-Airplane-Helicopter/dp/B09TDFVWHS/ref=sr_1_1?dib=eyJ2IjoiMSJ9.riuler2SJ2K370oVwQohtNzuSRoCNMr3AgKZDJKD89us8ngrWmuQdQl3ogluOg-ASMoJJ5PtQqXOHwWlzm9_BE894ZhAyBr1AwkwDSZmq8nsztUxRCW0BnSoIvykL-n9mWcwi0aQil2N_n5nMjHOHitjtOPNVAtV5IuiqRomjIccON42_1kX-URmIfOZaNwR8EbgpVzZsoStStY6ZJFoaAjrDcNI1TfKhpov36r8A6D5UW7KrFyGNrIV8tdYtGV00BkjCZVLSAL0vL5SR4PBucaMePTvVA3bQu5wYEkgSmw.j3O6RipRm9qIgwoU96EFSCHXXnMJBjUAicPNW96VEQA&amp;dib_tag=se&amp;keywords=3S+8400+mah&amp;qid=1756610025&amp;sr=8-1" xr:uid="{19E65730-6900-417B-BAE6-CAB9289FD747}"/>
-    <hyperlink ref="B25" r:id="rId8" display="Amazon" xr:uid="{CDAFC55C-E851-401E-BBCF-1C6A02C64874}"/>
-    <hyperlink ref="B13" r:id="rId9" xr:uid="{3112BEC5-0070-4734-A13C-033FA815C0C8}"/>
-    <hyperlink ref="B19" r:id="rId10" xr:uid="{E652C524-982E-4015-931D-A51BB57A61B0}"/>
+    <hyperlink ref="B21" r:id="rId4" display="https://www.amazon.ca/NVIDIA-Jetson-Orin-Nano-Developer/dp/B0BZJTQ5YP/ref=sr_1_5?dib=eyJ2IjoiMSJ9.oBPmo8N1125w9UZ8-xtxgBB0vzdg_OFiDKOJUmUak3KsGol2xTi80fCYUWqHlOGe2kAe8ESSo6BWqINztXDYxQeYiaTolbh4JB0c7Y3jwzqBn2JFR0HiK1FyJ5kyFpPhXSp1aJv5xMC--j8b-fNhdLSSJwvjbd0XY8EXhorkOxJFMnOfcD0O0oLoypf_Fx_o_Mmr-y09hK1oqRhDgOKDMI8MH5wdi7HBtWLImeM1blm4-70toRIjqXFsuk1DjbODSwJutIPBQJ3qrJjQuqE5pt5imxUwUY1I2YieMJwjEhU.iMrYs9zK_mCJTvqh5PRE7PjCeBtP2gORpf3H3tjRj9Q&amp;dib_tag=se&amp;keywords=jetson+orin+nano+dev+kit&amp;qid=1759703130&amp;sr=8-5" xr:uid="{1292E30F-6024-4A1A-B37C-1DA10F1BD571}"/>
+    <hyperlink ref="B22" r:id="rId5" xr:uid="{570B946F-A3F9-46CD-89E7-C74FEE892AE5}"/>
+    <hyperlink ref="B10" r:id="rId6" display="Amazon" xr:uid="{41208C38-E731-44F2-BEE2-61FCB8EB62DA}"/>
+    <hyperlink ref="B15" r:id="rId7" display="https://www.amazon.ca/DXF-Battery-Hardcase-Airplane-Helicopter/dp/B09TDFVWHS/ref=sr_1_1?dib=eyJ2IjoiMSJ9.riuler2SJ2K370oVwQohtNzuSRoCNMr3AgKZDJKD89us8ngrWmuQdQl3ogluOg-ASMoJJ5PtQqXOHwWlzm9_BE894ZhAyBr1AwkwDSZmq8nsztUxRCW0BnSoIvykL-n9mWcwi0aQil2N_n5nMjHOHitjtOPNVAtV5IuiqRomjIccON42_1kX-URmIfOZaNwR8EbgpVzZsoStStY6ZJFoaAjrDcNI1TfKhpov36r8A6D5UW7KrFyGNrIV8tdYtGV00BkjCZVLSAL0vL5SR4PBucaMePTvVA3bQu5wYEkgSmw.j3O6RipRm9qIgwoU96EFSCHXXnMJBjUAicPNW96VEQA&amp;dib_tag=se&amp;keywords=3S+8400+mah&amp;qid=1756610025&amp;sr=8-1" xr:uid="{19E65730-6900-417B-BAE6-CAB9289FD747}"/>
+    <hyperlink ref="B23" r:id="rId8" xr:uid="{CDAFC55C-E851-401E-BBCF-1C6A02C64874}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{3112BEC5-0070-4734-A13C-033FA815C0C8}"/>
+    <hyperlink ref="B17" r:id="rId10" xr:uid="{E652C524-982E-4015-931D-A51BB57A61B0}"/>
     <hyperlink ref="B7" r:id="rId11" xr:uid="{435C99FE-EDD2-4E84-983E-5B33DA420949}"/>
     <hyperlink ref="B8" r:id="rId12" xr:uid="{9D9F8FA0-0FB8-40F9-964C-907A1BB5FBE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
-  <drawing r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -1239,14 +1091,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="73decd86-39a4-49eb-910d-a9d7478bb842" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FBE23F23D6C404CAD5DE15B10DA803A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="173af77996ad3160ba67f97a1dc9a0a1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="73decd86-39a4-49eb-910d-a9d7478bb842" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac7655f4c6b06e1f724061c6ed122ee0" ns3:_="">
     <xsd:import namespace="73decd86-39a4-49eb-910d-a9d7478bb842"/>
@@ -1426,6 +1270,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="73decd86-39a4-49eb-910d-a9d7478bb842" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C9EC6FB-1CF2-4FAD-B830-F4943A84763F}">
   <ds:schemaRefs>
@@ -1435,22 +1287,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4BBE388-63B8-4E8B-9309-4F27288A6A4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="73decd86-39a4-49eb-910d-a9d7478bb842"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E58C759-CD66-46BE-BFED-9AE0DBCB8632}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1466,4 +1302,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4BBE388-63B8-4E8B-9309-4F27288A6A4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="73decd86-39a4-49eb-910d-a9d7478bb842"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>